<commit_message>
Added Browser,configReader,config properties file,Login test data file,updated LoginTest
</commit_message>
<xml_diff>
--- a/Testing_Project.com/src/test/resources/Test_Data/Login.xlsx
+++ b/Testing_Project.com/src/test/resources/Test_Data/Login.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>username</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>admin123</t>
+  </si>
+  <si>
+    <t>admin12</t>
   </si>
 </sst>
 </file>
@@ -37,15 +40,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -57,8 +59,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor theme="0"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -87,10 +89,10 @@
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -307,10 +309,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="27.5"/>
-    <col customWidth="1" min="2" max="2" width="31.13"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -326,6 +324,14 @@
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>